<commit_message>
simpen dulu ya sebelum di koding
</commit_message>
<xml_diff>
--- a/DATA TESTING & DATA UJI/datauji_mona_tanaman - Copy.xlsx
+++ b/DATA TESTING & DATA UJI/datauji_mona_tanaman - Copy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kickymaulana\Downloads\mona\knn_algorithm\DATA TESTING &amp; DATA UJI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF4A5479-2036-47C9-B70A-24371B5A75F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9E1592E-246C-4E32-9A75-06A1B8C292E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B37114CE-FFD3-4359-84AD-C162DBE58A15}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="97">
   <si>
     <t>nama</t>
   </si>
@@ -64,18 +64,6 @@
     <t>BAS TOMI ARDIANTO SITINJAK</t>
   </si>
   <si>
-    <t>BERNAD TOMSON SIMARE MARE</t>
-  </si>
-  <si>
-    <t>JULKIPLY TAMBA SIMANULLANG</t>
-  </si>
-  <si>
-    <t>Lamhot Naibaho</t>
-  </si>
-  <si>
-    <t>Lasman Simanjuntak</t>
-  </si>
-  <si>
     <t>email</t>
   </si>
   <si>
@@ -338,27 +326,6 @@
   </si>
   <si>
     <t>Kampung Dame</t>
-  </si>
-  <si>
-    <t>Pitta Pangaribuan</t>
-  </si>
-  <si>
-    <t>Sadar Turnip</t>
-  </si>
-  <si>
-    <t>Sahala Sirait</t>
-  </si>
-  <si>
-    <t>Kostan Silaen</t>
-  </si>
-  <si>
-    <t>Edihot Sinaga</t>
-  </si>
-  <si>
-    <t>Jampi Sitorus Pane</t>
-  </si>
-  <si>
-    <t>Sukarame</t>
   </si>
 </sst>
 </file>
@@ -729,7 +696,7 @@
   <dimension ref="A1:K81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -746,13 +713,13 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -770,25 +737,25 @@
         <v>3</v>
       </c>
       <c r="I1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
         <f ca="1">TEXT(RANDBETWEEN(1,9),"0")&amp;TEXT(RANDBETWEEN(0,999999999999999),"000000000000000")</f>
-        <v>7195603129897027</v>
+        <v>9587125215068726</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D2" s="4">
         <v>0.64</v>
@@ -806,25 +773,25 @@
         <v>24</v>
       </c>
       <c r="I2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="str">
-        <f t="shared" ref="A3:A16" ca="1" si="0">TEXT(RANDBETWEEN(1,9),"0")&amp;TEXT(RANDBETWEEN(0,999999999999999),"000000000000000")</f>
-        <v>5300272503649800</v>
+        <f t="shared" ref="A3:A6" ca="1" si="0">TEXT(RANDBETWEEN(1,9),"0")&amp;TEXT(RANDBETWEEN(0,999999999999999),"000000000000000")</f>
+        <v>6229912661845661</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D3" s="4">
         <v>0.8</v>
@@ -842,25 +809,25 @@
         <v>29</v>
       </c>
       <c r="I3" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2938041364303002</v>
+        <v>7107831043852049</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D4" s="4">
         <v>2</v>
@@ -878,25 +845,25 @@
         <v>73</v>
       </c>
       <c r="I4" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2902347768657083</v>
+        <v>3111708956294224</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D5" s="4">
         <v>1.6</v>
@@ -914,25 +881,25 @@
         <v>59</v>
       </c>
       <c r="I5" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>6443692189287713</v>
+        <v>6544848193525910</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D6" s="4">
         <v>0.48</v>
@@ -950,551 +917,141 @@
         <v>18</v>
       </c>
       <c r="I6" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>2327452335171949</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D7" s="4">
-        <v>0.4</v>
-      </c>
-      <c r="E7" s="4">
-        <v>26</v>
-      </c>
-      <c r="F7" s="4">
-        <v>26</v>
-      </c>
-      <c r="G7" s="4">
-        <v>15</v>
-      </c>
-      <c r="H7" s="4">
-        <v>15</v>
-      </c>
-      <c r="I7" t="s">
-        <v>100</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>98</v>
-      </c>
+      <c r="B7"/>
+      <c r="C7"/>
+      <c r="D7"/>
+      <c r="E7"/>
+      <c r="F7"/>
+      <c r="G7"/>
+      <c r="H7"/>
+      <c r="J7"/>
+      <c r="K7"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>7178625874953319</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D8" s="4">
-        <v>4</v>
-      </c>
-      <c r="E8" s="4">
-        <v>264</v>
-      </c>
-      <c r="F8" s="4">
-        <v>264</v>
-      </c>
-      <c r="G8" s="4">
-        <v>147</v>
-      </c>
-      <c r="H8" s="4">
-        <v>147</v>
-      </c>
-      <c r="I8" t="s">
-        <v>100</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>98</v>
-      </c>
+      <c r="B8"/>
+      <c r="C8"/>
+      <c r="D8"/>
+      <c r="E8"/>
+      <c r="F8"/>
+      <c r="G8"/>
+      <c r="H8"/>
+      <c r="J8"/>
+      <c r="K8"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>3889859813543861</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D9" s="4">
-        <v>3.6</v>
-      </c>
-      <c r="E9" s="4">
-        <v>238</v>
-      </c>
-      <c r="F9" s="4">
-        <v>238</v>
-      </c>
-      <c r="G9" s="4">
-        <v>132</v>
-      </c>
-      <c r="H9" s="4">
-        <v>132</v>
-      </c>
-      <c r="I9" t="s">
-        <v>100</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>98</v>
-      </c>
+      <c r="B9"/>
+      <c r="C9"/>
+      <c r="D9"/>
+      <c r="E9"/>
+      <c r="F9"/>
+      <c r="G9"/>
+      <c r="H9"/>
+      <c r="J9"/>
+      <c r="K9"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>9403370648534946</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D10" s="4">
-        <v>1</v>
-      </c>
-      <c r="E10" s="4">
-        <v>66</v>
-      </c>
-      <c r="F10" s="4">
-        <v>66</v>
-      </c>
-      <c r="G10" s="4">
-        <v>37</v>
-      </c>
-      <c r="H10" s="4">
-        <v>37</v>
-      </c>
-      <c r="I10" t="s">
-        <v>100</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>98</v>
-      </c>
+      <c r="B10"/>
+      <c r="C10"/>
+      <c r="D10"/>
+      <c r="E10"/>
+      <c r="F10"/>
+      <c r="G10"/>
+      <c r="H10"/>
+      <c r="J10"/>
+      <c r="K10"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>3320163289747275</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D11" s="4">
-        <v>2.4</v>
-      </c>
-      <c r="E11" s="4">
-        <v>220</v>
-      </c>
-      <c r="F11" s="4">
-        <v>220</v>
-      </c>
-      <c r="G11" s="4">
-        <v>144</v>
-      </c>
-      <c r="H11" s="4">
-        <v>144</v>
-      </c>
-      <c r="I11" t="s">
-        <v>107</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K11" s="3" t="s">
-        <v>98</v>
-      </c>
+      <c r="B11"/>
+      <c r="C11"/>
+      <c r="D11"/>
+      <c r="E11"/>
+      <c r="F11"/>
+      <c r="G11"/>
+      <c r="H11"/>
+      <c r="J11"/>
+      <c r="K11"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>2055423110811563</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D12" s="4">
-        <v>1.08</v>
-      </c>
-      <c r="E12" s="4">
-        <v>99</v>
-      </c>
-      <c r="F12" s="4">
-        <v>99</v>
-      </c>
-      <c r="G12" s="4">
-        <v>64</v>
-      </c>
-      <c r="H12" s="4">
-        <v>64</v>
-      </c>
-      <c r="I12" t="s">
-        <v>107</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K12" s="3" t="s">
-        <v>98</v>
-      </c>
+      <c r="B12"/>
+      <c r="C12"/>
+      <c r="D12"/>
+      <c r="E12"/>
+      <c r="F12"/>
+      <c r="G12"/>
+      <c r="H12"/>
+      <c r="J12"/>
+      <c r="K12"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>7281553052705466</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D13" s="4">
-        <v>0.96</v>
-      </c>
-      <c r="E13" s="4">
-        <v>88</v>
-      </c>
-      <c r="F13" s="4">
-        <v>88</v>
-      </c>
-      <c r="G13" s="4">
-        <v>57</v>
-      </c>
-      <c r="H13" s="4">
-        <v>57</v>
-      </c>
-      <c r="I13" t="s">
-        <v>107</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K13" s="3" t="s">
-        <v>98</v>
-      </c>
+      <c r="B13"/>
+      <c r="C13"/>
+      <c r="D13"/>
+      <c r="E13"/>
+      <c r="F13"/>
+      <c r="G13"/>
+      <c r="H13"/>
+      <c r="J13"/>
+      <c r="K13"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>6760540837453122</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D14" s="4">
-        <v>0.48</v>
-      </c>
-      <c r="E14" s="4">
-        <v>44</v>
-      </c>
-      <c r="F14" s="4">
-        <v>44</v>
-      </c>
-      <c r="G14" s="4">
-        <v>28</v>
-      </c>
-      <c r="H14" s="4">
-        <v>28</v>
-      </c>
-      <c r="I14" t="s">
-        <v>107</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K14" s="3" t="s">
-        <v>98</v>
-      </c>
+      <c r="B14"/>
+      <c r="C14"/>
+      <c r="D14"/>
+      <c r="E14"/>
+      <c r="F14"/>
+      <c r="G14"/>
+      <c r="H14"/>
+      <c r="J14"/>
+      <c r="K14"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>7441848714132504</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D15" s="4">
-        <v>0.6</v>
-      </c>
-      <c r="E15" s="4">
-        <v>55</v>
-      </c>
-      <c r="F15" s="4">
-        <v>55</v>
-      </c>
-      <c r="G15" s="4">
-        <v>36</v>
-      </c>
-      <c r="H15" s="4">
-        <v>36</v>
-      </c>
-      <c r="I15" t="s">
-        <v>107</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K15" s="3" t="s">
-        <v>98</v>
-      </c>
+      <c r="B15"/>
+      <c r="C15"/>
+      <c r="D15"/>
+      <c r="E15"/>
+      <c r="F15"/>
+      <c r="G15"/>
+      <c r="H15"/>
+      <c r="J15"/>
+      <c r="K15"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>7462483394073554</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D16" s="4">
-        <v>1.44</v>
-      </c>
-      <c r="E16" s="4">
-        <v>132</v>
-      </c>
-      <c r="F16" s="4">
-        <v>132</v>
-      </c>
-      <c r="G16" s="4">
-        <v>86</v>
-      </c>
-      <c r="H16" s="4">
-        <v>86</v>
-      </c>
-      <c r="I16" t="s">
-        <v>107</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K16" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B17"/>
-      <c r="C17"/>
-      <c r="D17"/>
-      <c r="E17"/>
-      <c r="F17"/>
-      <c r="G17"/>
-      <c r="H17"/>
-      <c r="J17"/>
-      <c r="K17"/>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B18"/>
-      <c r="C18"/>
-      <c r="D18"/>
-      <c r="E18"/>
-      <c r="F18"/>
-      <c r="G18"/>
-      <c r="H18"/>
-      <c r="J18"/>
-      <c r="K18"/>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B19"/>
-      <c r="C19"/>
-      <c r="D19"/>
-      <c r="E19"/>
-      <c r="F19"/>
-      <c r="G19"/>
-      <c r="H19"/>
-      <c r="J19"/>
-      <c r="K19"/>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B20"/>
-      <c r="C20"/>
-      <c r="D20"/>
-      <c r="E20"/>
-      <c r="F20"/>
-      <c r="G20"/>
-      <c r="H20"/>
-      <c r="J20"/>
-      <c r="K20"/>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B21"/>
-      <c r="C21"/>
-      <c r="D21"/>
-      <c r="E21"/>
-      <c r="F21"/>
-      <c r="G21"/>
-      <c r="H21"/>
-      <c r="J21"/>
-      <c r="K21"/>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B22"/>
-      <c r="C22"/>
-      <c r="D22"/>
-      <c r="E22"/>
-      <c r="F22"/>
-      <c r="G22"/>
-      <c r="H22"/>
-      <c r="J22"/>
-      <c r="K22"/>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B23"/>
-      <c r="C23"/>
-      <c r="D23"/>
-      <c r="E23"/>
-      <c r="F23"/>
-      <c r="G23"/>
-      <c r="H23"/>
-      <c r="J23"/>
-      <c r="K23"/>
-    </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B24"/>
-      <c r="C24"/>
-      <c r="D24"/>
-      <c r="E24"/>
-      <c r="F24"/>
-      <c r="G24"/>
-      <c r="H24"/>
-      <c r="J24"/>
-      <c r="K24"/>
-    </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B25"/>
-      <c r="C25"/>
-      <c r="D25"/>
-      <c r="E25"/>
-      <c r="F25"/>
-      <c r="G25"/>
-      <c r="H25"/>
-      <c r="J25"/>
-      <c r="K25"/>
-    </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B26"/>
-      <c r="C26"/>
-      <c r="D26"/>
-      <c r="E26"/>
-      <c r="F26"/>
-      <c r="G26"/>
-      <c r="H26"/>
-      <c r="J26"/>
-      <c r="K26"/>
-    </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B27"/>
-      <c r="C27"/>
-      <c r="D27"/>
-      <c r="E27"/>
-      <c r="F27"/>
-      <c r="G27"/>
-      <c r="H27"/>
-      <c r="J27"/>
-      <c r="K27"/>
-    </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B28"/>
-      <c r="C28"/>
-      <c r="D28"/>
-      <c r="E28"/>
-      <c r="F28"/>
-      <c r="G28"/>
-      <c r="H28"/>
-      <c r="J28"/>
-      <c r="K28"/>
-    </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B29"/>
-      <c r="C29"/>
-      <c r="D29"/>
-      <c r="E29"/>
-      <c r="F29"/>
-      <c r="G29"/>
-      <c r="H29"/>
-      <c r="J29"/>
-      <c r="K29"/>
-    </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B30"/>
-      <c r="C30"/>
-      <c r="D30"/>
-      <c r="E30"/>
-      <c r="F30"/>
-      <c r="G30"/>
-      <c r="H30"/>
-      <c r="J30"/>
-      <c r="K30"/>
-    </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B31"/>
-      <c r="C31"/>
-      <c r="D31"/>
-      <c r="E31"/>
-      <c r="F31"/>
-      <c r="G31"/>
-      <c r="H31"/>
-      <c r="J31"/>
-      <c r="K31"/>
-    </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B32"/>
-      <c r="C32"/>
-      <c r="D32"/>
-      <c r="E32"/>
-      <c r="F32"/>
-      <c r="G32"/>
-      <c r="H32"/>
-      <c r="J32"/>
-      <c r="K32"/>
-    </row>
+      <c r="B16"/>
+      <c r="C16"/>
+      <c r="D16"/>
+      <c r="E16"/>
+      <c r="F16"/>
+      <c r="G16"/>
+      <c r="H16"/>
+      <c r="J16"/>
+      <c r="K16"/>
+    </row>
+    <row r="17" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="18" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="19" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="20" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="21" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="22" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="23" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="24" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="25" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="26" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="27" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="28" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="29" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="30" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="31" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="32" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="33" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="34" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="35" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -1547,7 +1104,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="J2" r:id="rId1" xr:uid="{CF04E591-0111-432B-BDBC-3DCF54C98201}"/>
-    <hyperlink ref="J3:J16" r:id="rId2" display="email@gmail.com" xr:uid="{67ED74BA-2F9E-4E6C-A25B-171CC4EA0A7F}"/>
+    <hyperlink ref="J3:J6" r:id="rId2" display="email@gmail.com" xr:uid="{67ED74BA-2F9E-4E6C-A25B-171CC4EA0A7F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -1569,138 +1126,138 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C11" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C13" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C15" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C16" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C17" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -1708,221 +1265,221 @@
         <v>3216191311800010</v>
       </c>
       <c r="C18" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C19" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C20" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C21" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C22" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C23" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C24" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C25" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C26" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C27" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C29" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C30" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C31" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C32" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C33" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="34" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C34" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="35" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C35" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="36" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C36" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="37" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C37" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="38" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C38" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="39" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C39" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="40" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C40" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="41" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C41" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="42" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C42" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="43" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C43" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="44" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C44" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="45" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C45" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="46" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C46" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="47" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C47" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="48" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C48" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="49" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C49" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="50" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C50" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="51" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C51" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="52" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C52" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="53" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C53" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="54" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C54" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="55" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C55" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="56" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C56" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="57" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C57" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="58" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C58" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="59" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C59" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="60" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C60" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>